<commit_message>
tabela pronta dos produtos que mais cresceram
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,22 +456,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Qnt-Normal</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Qnt-FULL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Media-Preco</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Qnt-Normal</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Qnt-FULL</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Mediana-Preco</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Media-Vendas</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana-Vendas</t>
         </is>
       </c>
     </row>
@@ -493,20 +503,30 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>17.105 resultado</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>233 resultado</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1491.157894736842</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1235</v>
       </c>
     </row>
     <row r="3">
@@ -527,24 +547,30 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>38.5</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>10.821 resultado</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10.820 resultado</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>44 resultado</t>
         </is>
       </c>
+      <c r="G3" t="n">
+        <v>126.8235294117647</v>
+      </c>
       <c r="H3" t="n">
-        <v>171.5</v>
+        <v>135</v>
+      </c>
+      <c r="I3" t="n">
+        <v>89.76470588235294</v>
+      </c>
+      <c r="J3" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -565,20 +591,30 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>600 resultado</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>74 resultado</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>66.31578947368421</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="I4" t="n">
+        <v>585.421052631579</v>
+      </c>
+      <c r="J4" t="n">
+        <v>460</v>
       </c>
     </row>
     <row r="5">
@@ -599,20 +635,30 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2.788 resultado</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>42 resultado</t>
+        </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>253.3571428571429</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>172</v>
+      </c>
+      <c r="I5" t="n">
+        <v>310.4285714285714</v>
+      </c>
+      <c r="J5" t="n">
+        <v>227.5</v>
       </c>
     </row>
     <row r="6">
@@ -633,20 +679,30 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>18.756 resultado</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>327 resultado</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>55.63157894736842</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1968.526315789474</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1337</v>
       </c>
     </row>
     <row r="7">
@@ -667,20 +723,30 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1.108 resultado</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>52 resultado</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>196.7222222222222</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>139</v>
+      </c>
+      <c r="I7" t="n">
+        <v>29</v>
+      </c>
+      <c r="J7" t="n">
+        <v>9.5</v>
       </c>
     </row>
     <row r="8">
@@ -701,20 +767,30 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2.382 resultado</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>36 resultado</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>64.07692307692308</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1541.153846153846</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1108</v>
       </c>
     </row>
     <row r="9">
@@ -735,20 +811,30 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>150.268 resultado</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3.166 resultado</t>
+        </is>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>61.68421052631579</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14095.57894736842</v>
+      </c>
+      <c r="J9" t="n">
+        <v>6781</v>
       </c>
     </row>
     <row r="10">
@@ -769,20 +855,30 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>679 resultado</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NaoTem</t>
+        </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>588.1666666666666</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>569</v>
+      </c>
+      <c r="I10" t="n">
+        <v>180.5</v>
+      </c>
+      <c r="J10" t="n">
+        <v>97.5</v>
       </c>
     </row>
     <row r="11">
@@ -803,20 +899,30 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-05-20 15:56:48</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
+          <t>2022-05-20 16:23:08</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>38.178 resultado</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>500 resultado</t>
+        </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>78.16666666666667</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>47.5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2699.666666666667</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2332.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
concertando bug procurar nome produto - p para h3
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Mediana-Vendas</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>GoogleTrends</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -503,12 +508,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
+          <t>2022-05-20 19:23:22</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17.105 resultado</t>
+          <t>17.113 resultado</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -517,16 +522,21 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>93</v>
+        <v>85.33333333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="I2" t="n">
-        <v>1491.157894736842</v>
+        <v>3381</v>
       </c>
       <c r="J2" t="n">
-        <v>1235</v>
+        <v>4454</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=bbs airsoft</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -547,12 +557,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
+          <t>2022-05-20 19:23:22</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10.821 resultado</t>
+          <t>10.822 resultado</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -561,16 +571,21 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>126.8235294117647</v>
+        <v>35</v>
       </c>
       <c r="H3" t="n">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="I3" t="n">
-        <v>89.76470588235294</v>
+        <v>181</v>
       </c>
       <c r="J3" t="n">
-        <v>56</v>
+        <v>200</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=alvo tiro</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -591,30 +606,31 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>600 resultado</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>74 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>66.31578947368421</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>585.421052631579</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>460</v>
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -635,30 +651,31 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2.788 resultado</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>42 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>253.3571428571429</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>310.4285714285714</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>227.5</v>
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -679,30 +696,31 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>18.756 resultado</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>327 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>55.63157894736842</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1968.526315789474</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>1337</v>
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -723,30 +741,31 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1.108 resultado</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>52 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>196.7222222222222</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>9.5</v>
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -767,30 +786,31 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2.382 resultado</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>36 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>64.07692307692308</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1541.153846153846</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>1108</v>
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -811,30 +831,31 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>150.268 resultado</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>3.166 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>61.68421052631579</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>14095.57894736842</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>6781</v>
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -855,30 +876,31 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>679 resultado</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NaoTem</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>588.1666666666666</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>569</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>180.5</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>97.5</v>
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -899,30 +921,31 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-05-20 16:23:08</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>38.178 resultado</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>500 resultado</t>
-        </is>
+          <t>2022-05-20 19:23:22</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>78.16666666666667</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>47.5</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>2699.666666666667</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>2332.5</v>
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionado wait until e round
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>85.33333333333333</v>
+        <v>85.33329999999999</v>
       </c>
       <c r="H2" t="n">
         <v>89</v>
@@ -557,7 +557,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -651,7 +651,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -696,7 +696,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -741,7 +741,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -786,7 +786,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -831,7 +831,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -876,7 +876,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -921,7 +921,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-05-20 19:23:22</t>
+          <t>2022-05-20 19:31:54</t>
         </is>
       </c>
       <c r="E11" t="n">

</xml_diff>

<commit_message>
puxando dados de todas tendencias
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,163 +451,168 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Qnt-Normal</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Qnt-FULL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Media-Preco</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana-Preco</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Media-Vendas</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana-Vendas</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>GoogleTrends</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Tendencia</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>scrapy_datetime</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Qnt-Normal</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Qnt-FULL</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Media-Preco</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Mediana-Preco</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Media-Vendas</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Mediana-Vendas</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>GoogleTrends</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bbs airsoft</t>
+          <t>meia beach tennis</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/bbs-airsoft</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>17.113 resultado</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>233 resultado</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/meia-beach-tennis</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>85.33329999999999</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>3381</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4454</v>
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=bbs airsoft</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>alvo tiro</t>
+          <t>bandana tubular</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/alvo-tiro</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10.822 resultado</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>44 resultado</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/bandana-tubular</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>181</v>
-      </c>
-      <c r="J3" t="n">
-        <v>200</v>
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=alvo tiro</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cano 5 5</t>
+          <t>roupa camuflada</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/cano-5-5</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/roupa-camuflada</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -624,35 +629,40 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>coldre ts9</t>
+          <t>bicicleta triciclo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/coldre-ts9</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/bicicleta-triciclo</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -669,35 +679,40 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>bandagem</t>
+          <t>camelbak</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/bandagem</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/camelbak</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -714,35 +729,40 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>tenis society masculino</t>
+          <t>bermuda termica masculina</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/tenis-society-masculino</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/bermuda-termica-masculina</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -759,35 +779,40 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>7º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bermuda termica masculina</t>
+          <t>arpao pesca</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/bermuda-termica-masculina</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/arpao-pesca</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -804,35 +829,40 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>kit academia</t>
+          <t>kit sobrevivencia completo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/kit-academia</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/kit-sobrevivencia-completo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -849,35 +879,40 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>9º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>arpao pesca</t>
+          <t>garrafa personalizada</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/arpao-pesca</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/garrafa-personalizada</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -894,35 +929,40 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>10º MAIOR CRESCIMENTO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>joelheira</t>
+          <t>quechua</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://lista.mercadolivre.com.br/joelheira</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2022-05-20 19:31:54</t>
-        </is>
+          <t>https://lista.mercadolivre.com.br/quechua</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -939,12 +979,2019 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>balaclava</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/balaclava</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>colchonete</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/colchonete</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>squeeze</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/squeeze</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>4º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>garrafa agua</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/garrafa-agua</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>5º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>blade 98 305gr</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/blade-98-305gr</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>6º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sapatilha beach tennis</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/sapatilha-beach-tennis</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>7º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>casual</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/casual</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>8º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>academia</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/academia</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>9º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>colchonete solteiro</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/colchonete-solteiro</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>colete salva vidas</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/colete-salva-vidas</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>tatame academia</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/tatame-academia</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>12º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>bomba pcp</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bomba-pcp</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>13º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>bermuda ciclismo</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bermuda-ciclismo</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>caneleira</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/caneleira</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>15º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>kit funcional futebol</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/kit-funcional-futebol</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>16º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>bola</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bola</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>17º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>luneta victoptics</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/luneta-victoptics</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>18º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>piso borracha academia</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/piso-borracha-academia</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>19º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>esteira eletrica movement residencial r4 110v</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/esteira-eletrica-movement-residencial-r4-110v</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>20º MAIS DESEJADA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>aisoft bbs</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/aisoft-bbs</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>chumbinho 5 5</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/chumbinho-5-5</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>colchonete casal</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/colchonete-casal</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>3º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mira red dot</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/mira-red-dot</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>4º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>red dot</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/red-dot</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>5º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>bandana balaclava</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bandana-balaclava</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>6º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>decathlon</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/decathlon</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>7º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mira laser</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/mira-laser</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>8º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>garrafa de agua</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/garrafa-de-agua</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>9º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>bretelle ciclismo</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bretelle-ciclismo</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>10º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>coldres taticos</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/coldres-taticos</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>11º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>coldre</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/coldre</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>12º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>bandagem elastica</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bandagem-elastica</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>13º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>garrafinha de agua</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/garrafinha-de-agua</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>14º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>squeeze termico</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/squeeze-termico</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>15º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>abafador eletronico</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/abafador-eletronico</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>16º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>defesa pessoal</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/defesa-pessoal</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>bomba de ar</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/bomba-de-ar</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>18º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>munhequeira crossfit</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/munhequeira-crossfit</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>19º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>garrafinha termica</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/garrafinha-termica</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>20º MAIS POPULAR</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>camisa nike masculina</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://lista.mercadolivre.com.br/camisa-nike-masculina</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>2022-05-20 22:41:47</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
tabela de uma categoria concluida
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,11 +486,6 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Tendencia</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
           <t>scrapy_datetime</t>
         </is>
       </c>
@@ -511,37 +506,36 @@
           <t>https://lista.mercadolivre.com.br/meia-beach-tennis</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>247 resultado</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>105 resultado</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>262.67</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=meia beach tennis</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -561,37 +555,36 @@
           <t>https://lista.mercadolivre.com.br/bandana-tubular</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1.866 resultado</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>15 resultado</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1205</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>695</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=bandana tubular</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -611,37 +604,36 @@
           <t>https://lista.mercadolivre.com.br/roupa-camuflada</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>897 resultado</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>17 resultado</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=roupa camuflada</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -661,37 +653,36 @@
           <t>https://lista.mercadolivre.com.br/bicicleta-triciclo</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>893 resultado</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>9 resultado</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1039.67</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>737</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1196</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1639</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=bicicleta triciclo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -711,37 +702,36 @@
           <t>https://lista.mercadolivre.com.br/camelbak</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>8.220 resultado</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>148 resultado</t>
+        </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1215</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>514</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=camelbak</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -761,37 +751,36 @@
           <t>https://lista.mercadolivre.com.br/bermuda-termica-masculina</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2.382 resultado</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>36 resultado</t>
+        </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1627.33</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=bermuda termica masculina</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -811,37 +800,36 @@
           <t>https://lista.mercadolivre.com.br/arpao-pesca</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>679 resultado</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NaoTem</t>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>526</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=arpao pesca</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -861,37 +849,36 @@
           <t>https://lista.mercadolivre.com.br/kit-sobrevivencia-completo</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>42.138 resultado</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>401 resultado</t>
+        </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>275.67</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=kit sobrevivencia completo</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -911,37 +898,36 @@
           <t>https://lista.mercadolivre.com.br/garrafa-personalizada</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2.830 resultado</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>32 resultado</t>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=garrafa personalizada</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -961,37 +947,36 @@
           <t>https://lista.mercadolivre.com.br/quechua</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1.751 resultado</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1 resultado</t>
+        </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>149.67</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=quechua</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1011,37 +996,36 @@
           <t>https://lista.mercadolivre.com.br/balaclava</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7.236 resultado</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>132 resultado</t>
+        </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>29.33</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1458</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=balaclava</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1061,37 +1045,36 @@
           <t>https://lista.mercadolivre.com.br/colchonete</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>17.508 resultado</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>259 resultado</t>
+        </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>39.67</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>32307</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>13580</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://trends.google.com.br/trends/explore?geo=BR&amp;q=colchonete</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1119,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1164,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1236,12 +1209,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1286,12 +1254,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1299,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1344,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1436,12 +1389,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1486,12 +1434,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1536,12 +1479,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1586,12 +1524,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1636,12 +1569,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1614,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1736,12 +1659,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1786,12 +1704,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1836,12 +1749,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1886,12 +1794,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1839,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -1986,12 +1884,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2036,12 +1929,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2086,12 +1974,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2136,12 +2019,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2186,12 +2064,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2236,12 +2109,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2286,12 +2154,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2336,12 +2199,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2386,12 +2244,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2289,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2486,12 +2334,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2536,12 +2379,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2586,12 +2424,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2636,12 +2469,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2686,12 +2514,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2736,12 +2559,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2786,12 +2604,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2836,12 +2649,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2886,12 +2694,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2936,12 +2739,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2784,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>2022-05-20 22:41:47</t>
+          <t>2022-05-21 08:45:30</t>
         </is>
       </c>
     </row>

</xml_diff>